<commit_message>
Dataset_1G added for testing
</commit_message>
<xml_diff>
--- a/training/training_timesheet.xlsx
+++ b/training/training_timesheet.xlsx
@@ -1074,7 +1074,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1576,6 +1576,552 @@
         <v>0.9818982926194322</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" t="n">
+        <v>8.037410736083984</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.9009041786193848</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.9038553721632818</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.8642713813112477</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.8632959663119331</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>2</v>
+      </c>
+      <c r="B23" t="n">
+        <v>17.80628418922424</v>
+      </c>
+      <c r="C23" t="n">
+        <v>9.768873453140259</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.9342758655548096</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.9317103189859292</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.8955077709887093</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.89482506946225</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>3</v>
+      </c>
+      <c r="B24" t="n">
+        <v>26.69517970085144</v>
+      </c>
+      <c r="C24" t="n">
+        <v>8.888895511627197</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.9247410893440247</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.9290847545054026</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.8876495648344066</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.8862864352204776</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>4</v>
+      </c>
+      <c r="B25" t="n">
+        <v>35.97301006317139</v>
+      </c>
+      <c r="C25" t="n">
+        <v>9.277830362319946</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.959855318069458</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.9572491923417846</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.9222882247224139</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.9222511348001811</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>5</v>
+      </c>
+      <c r="B26" t="n">
+        <v>44.3629789352417</v>
+      </c>
+      <c r="C26" t="n">
+        <v>8.389968872070312</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.9638336300849915</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.9607068603829316</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.9259423637818004</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.9253000781939975</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>6</v>
+      </c>
+      <c r="B27" t="n">
+        <v>52.88276696205139</v>
+      </c>
+      <c r="C27" t="n">
+        <v>8.519788026809692</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.9624527096748352</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.9631393028274935</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.9259345001925611</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.9267034133505136</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>7</v>
+      </c>
+      <c r="B28" t="n">
+        <v>62.56203389167786</v>
+      </c>
+      <c r="C28" t="n">
+        <v>9.679266929626465</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.9640966653823853</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.9616812555574823</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.9252630152870445</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.9236578548190372</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>8</v>
+      </c>
+      <c r="B29" t="n">
+        <v>73.32969045639038</v>
+      </c>
+      <c r="C29" t="n">
+        <v>10.76765656471252</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.9319414496421814</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.9387156493625052</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.898761260631326</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.8970461895495352</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>9</v>
+      </c>
+      <c r="B30" t="n">
+        <v>82.04559350013733</v>
+      </c>
+      <c r="C30" t="n">
+        <v>8.715903043746948</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.9741575121879578</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.972389452267386</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.9722806524280484</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.9722140580229934</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>10</v>
+      </c>
+      <c r="B31" t="n">
+        <v>90.77180194854736</v>
+      </c>
+      <c r="C31" t="n">
+        <v>8.726208448410034</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.9760973453521729</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.9756835050505298</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.9732429083582714</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.9739777117311195</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>11</v>
+      </c>
+      <c r="B32" t="n">
+        <v>100.0763611793518</v>
+      </c>
+      <c r="C32" t="n">
+        <v>9.304559230804443</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.9740259647369385</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.971767023505224</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.9728566953711947</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.9718508223790493</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>12</v>
+      </c>
+      <c r="B33" t="n">
+        <v>108.8250782489777</v>
+      </c>
+      <c r="C33" t="n">
+        <v>8.748717069625854</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.9755712747573853</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.97405812988468</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.9743299476204527</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.9740008877594032</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>13</v>
+      </c>
+      <c r="B34" t="n">
+        <v>117.0536303520203</v>
+      </c>
+      <c r="C34" t="n">
+        <v>8.228552103042603</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.9760644435882568</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.9737320709625401</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.9740349246244088</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.9732360897635419</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>14</v>
+      </c>
+      <c r="B35" t="n">
+        <v>126.663524389267</v>
+      </c>
+      <c r="C35" t="n">
+        <v>9.609894037246704</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.9765576124191284</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.976099714504825</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.9754770032127669</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.9756446323668319</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>15</v>
+      </c>
+      <c r="B36" t="n">
+        <v>135.897049665451</v>
+      </c>
+      <c r="C36" t="n">
+        <v>9.233525276184082</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.971329927444458</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.9709969823862185</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.9706319419241851</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.9704154821911015</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>16</v>
+      </c>
+      <c r="B37" t="n">
+        <v>144.0664365291595</v>
+      </c>
+      <c r="C37" t="n">
+        <v>8.169386863708496</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.9687325358390808</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.969710145939751</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.9694352366053616</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.9688816832119176</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>17</v>
+      </c>
+      <c r="B38" t="n">
+        <v>152.2339911460876</v>
+      </c>
+      <c r="C38" t="n">
+        <v>8.167554616928101</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.9661351442337036</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.9655260876826288</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.9617594163118518</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.9601438496307407</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>18</v>
+      </c>
+      <c r="B39" t="n">
+        <v>160.7514872550964</v>
+      </c>
+      <c r="C39" t="n">
+        <v>8.517496109008789</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.9788591265678406</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.9780127278479415</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.978218863794879</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.9780014459550754</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>19</v>
+      </c>
+      <c r="B40" t="n">
+        <v>171.4699847698212</v>
+      </c>
+      <c r="C40" t="n">
+        <v>10.71849751472473</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.9827058911323547</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.9816476376908092</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.980898479912813</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.9810578176394261</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>20</v>
+      </c>
+      <c r="B41" t="n">
+        <v>180.6203641891479</v>
+      </c>
+      <c r="C41" t="n">
+        <v>9.150379419326782</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.9794509410858154</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.977603868229227</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.9768589411552572</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.9762675116853456</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>1</v>
+      </c>
+      <c r="B42" t="n">
+        <v>20.5004358291626</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.9069867134094238</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.9110572373172203</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.8703144659650774</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.8709239189736855</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>2</v>
+      </c>
+      <c r="B43" t="n">
+        <v>44.49518322944641</v>
+      </c>
+      <c r="C43" t="n">
+        <v>23.99474740028381</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.9361499547958374</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.9370535028960167</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.8979039293265859</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.8990548970545544</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>3</v>
+      </c>
+      <c r="B44" t="n">
+        <v>67.79964804649353</v>
+      </c>
+      <c r="C44" t="n">
+        <v>23.30446481704712</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.9507151246070862</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.9513855397267067</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.9118300609374642</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.9128254086923384</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>4</v>
+      </c>
+      <c r="B45" t="n">
+        <v>92.18682742118835</v>
+      </c>
+      <c r="C45" t="n">
+        <v>24.38717937469482</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.9635705947875977</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.9625932551729826</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.9270077892056477</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.9273513163863312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>